<commit_message>
Updates pin layput, adding XLR mapping and consolidated RTD pins
</commit_message>
<xml_diff>
--- a/Design diagrams/Relay and Pin Layout.xlsx
+++ b/Design diagrams/Relay and Pin Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomatedBrewery\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AutomatedBrewery\Design diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,6 +15,8 @@
     <sheet name="Relays" sheetId="1" r:id="rId1"/>
     <sheet name="GPIO Pins" sheetId="2" r:id="rId2"/>
     <sheet name="SPI Addresses" sheetId="3" r:id="rId3"/>
+    <sheet name="XLR Mapping" sheetId="4" r:id="rId4"/>
+    <sheet name="RTD Pins" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="198">
   <si>
     <t>Relay</t>
   </si>
@@ -358,9 +360,6 @@
     <t>Temp 1 SDI</t>
   </si>
   <si>
-    <t>Temp 1 CS1 (HLT)</t>
-  </si>
-  <si>
     <t>MCP23017-3</t>
   </si>
   <si>
@@ -505,9 +504,6 @@
     <t>Temp 2 SDO</t>
   </si>
   <si>
-    <t>Temp 2 CS (BLK)</t>
-  </si>
-  <si>
     <t>Temp 2 SCLK</t>
   </si>
   <si>
@@ -536,6 +532,96 @@
   </si>
   <si>
     <t>ADC</t>
+  </si>
+  <si>
+    <t>Alarm</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>XLR Color</t>
+  </si>
+  <si>
+    <t>RTD Color</t>
+  </si>
+  <si>
+    <t>Valve Color</t>
+  </si>
+  <si>
+    <t>Gold/Bare</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Volume Wire</t>
+  </si>
+  <si>
+    <t>Flow Wire</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>MCP23017 Bus</t>
+  </si>
+  <si>
+    <t>csPin</t>
+  </si>
+  <si>
+    <t>misoPin</t>
+  </si>
+  <si>
+    <t>mosiPin</t>
+  </si>
+  <si>
+    <t>clkPin</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>MLT</t>
+  </si>
+  <si>
+    <t>BLK</t>
+  </si>
+  <si>
+    <t>0x21</t>
+  </si>
+  <si>
+    <t>Temp 2 CS (HLT)</t>
+  </si>
+  <si>
+    <t>Temp 1 CS1 (BLK)</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>IO Pin #</t>
+  </si>
+  <si>
+    <t>MCP23017-3 (0x21)</t>
+  </si>
+  <si>
+    <t>TEST123</t>
   </si>
 </sst>
 </file>
@@ -878,13 +964,13 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -923,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -940,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +1043,7 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,6 +1059,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
+      <c r="E6" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1048,7 +1137,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1057,7 +1146,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1106,24 +1195,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL22"/>
+  <dimension ref="A1:AV25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1144,26 +1234,32 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
-      <c r="U1" s="2" t="s">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="Y1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
-      <c r="AD1" s="2" t="s">
-        <v>111</v>
-      </c>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL1" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1188,62 +1284,98 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
+      <c r="K2" t="s">
+        <v>194</v>
+      </c>
       <c r="L2" t="s">
         <v>7</v>
       </c>
       <c r="M2" t="s">
+        <v>195</v>
+      </c>
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
+        <v>195</v>
+      </c>
+      <c r="S2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>9</v>
       </c>
       <c r="U2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" t="s">
-        <v>9</v>
+        <v>194</v>
+      </c>
+      <c r="X2" t="s">
+        <v>194</v>
       </c>
       <c r="Y2" t="s">
         <v>7</v>
       </c>
       <c r="Z2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AA2" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>9</v>
       </c>
       <c r="AD2" t="s">
         <v>7</v>
       </c>
       <c r="AE2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AF2" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>9</v>
       </c>
       <c r="AH2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL2" t="s">
         <v>7</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AM2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN2" t="s">
         <v>8</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AO2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AP2" t="s">
+        <v>195</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1271,66 +1403,84 @@
       <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" t="str">
+      <c r="M3">
+        <v>8</v>
+      </c>
+      <c r="N3" t="str">
         <f>"GPB"&amp;L3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="N3" s="5" t="str">
+      <c r="O3" s="5" t="str">
         <f>"Valve "&amp;L3&amp;" Positive Out"</f>
         <v>Valve 1 Positive Out</v>
       </c>
-      <c r="P3">
-        <f>P4+1</f>
+      <c r="Q3">
+        <f>Q4+1</f>
         <v>28</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3">
+        <v>7</v>
+      </c>
+      <c r="S3" t="s">
         <v>70</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="U3">
+      <c r="Y3">
         <v>1</v>
       </c>
-      <c r="V3" t="str">
-        <f>"GPB"&amp;U3-1</f>
+      <c r="Z3">
+        <v>8</v>
+      </c>
+      <c r="AA3" t="str">
+        <f>"GPB"&amp;Y3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="W3" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y3">
-        <f>Y4+1</f>
+      <c r="AB3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD3">
+        <f>AD4+1</f>
         <v>28</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AE3">
+        <v>7</v>
+      </c>
+      <c r="AF3" t="s">
         <v>70</v>
       </c>
-      <c r="AA3" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD3">
+      <c r="AG3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AL3">
         <v>1</v>
       </c>
-      <c r="AE3" t="str">
-        <f>"GPB"&amp;AD3-1</f>
+      <c r="AM3">
+        <v>8</v>
+      </c>
+      <c r="AN3" t="str">
+        <f>"GPB"&amp;AL3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="AF3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH3">
-        <f>AH4+1</f>
+      <c r="AO3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP3">
+        <v>7</v>
+      </c>
+      <c r="AQ3">
+        <f>AQ4+1</f>
         <v>28</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AS3" t="s">
         <v>70</v>
       </c>
-      <c r="AJ3" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT3" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>3</v>
@@ -1361,68 +1511,86 @@
         <f>L3+1</f>
         <v>2</v>
       </c>
-      <c r="M4" t="str">
-        <f t="shared" ref="M4:M10" si="0">"GPB"&amp;L4-1</f>
+      <c r="M4">
+        <v>9</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ref="N4:N10" si="0">"GPB"&amp;L4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="N4" s="5" t="str">
-        <f t="shared" ref="N4:N10" si="1">"Valve "&amp;L4&amp;" Positive Out"</f>
+      <c r="O4" s="5" t="str">
+        <f t="shared" ref="O4:O10" si="1">"Valve "&amp;L4&amp;" Positive Out"</f>
         <v>Valve 2 Positive Out</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P15" si="2">P5+1</f>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q15" si="2">Q5+1</f>
         <v>27</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4" t="s">
         <v>71</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="T4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="U4">
-        <f>U3+1</f>
+      <c r="Y4">
+        <f>Y3+1</f>
         <v>2</v>
       </c>
-      <c r="V4" t="str">
-        <f t="shared" ref="V4:V10" si="3">"GPB"&amp;U4-1</f>
+      <c r="Z4">
+        <v>9</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" ref="AA4:AA10" si="3">"GPB"&amp;Y4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="W4" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y4">
-        <f t="shared" ref="Y4:Y15" si="4">Y5+1</f>
+      <c r="AB4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" ref="AD4:AD15" si="4">AD5+1</f>
         <v>27</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AE4">
+        <v>6</v>
+      </c>
+      <c r="AF4" t="s">
         <v>71</v>
       </c>
-      <c r="AA4" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="AD4">
-        <f>AD3+1</f>
+      <c r="AG4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL4">
+        <f>AL3+1</f>
         <v>2</v>
       </c>
-      <c r="AE4" t="str">
-        <f t="shared" ref="AE4:AE10" si="5">"GPB"&amp;AD4-1</f>
+      <c r="AM4">
+        <v>9</v>
+      </c>
+      <c r="AN4" t="str">
+        <f t="shared" ref="AN4:AN10" si="5">"GPB"&amp;AL4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="AF4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH4">
-        <f t="shared" ref="AH4:AH15" si="6">AH5+1</f>
+      <c r="AO4" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP4">
+        <v>6</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" ref="AQ4:AQ15" si="6">AQ5+1</f>
         <v>27</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AS4" t="s">
         <v>71</v>
       </c>
-      <c r="AJ4" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT4" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A22" si="7">A4+2</f>
         <v>5</v>
@@ -1453,68 +1621,86 @@
         <f t="shared" ref="L5:L16" si="9">L4+1</f>
         <v>3</v>
       </c>
-      <c r="M5" t="str">
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5" t="str">
         <f t="shared" si="0"/>
         <v>GPB2</v>
       </c>
-      <c r="N5" s="5" t="str">
+      <c r="O5" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 3 Positive Out</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5" t="s">
         <v>72</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="T5" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="U5">
-        <f t="shared" ref="U5:U16" si="10">U4+1</f>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y16" si="10">Y4+1</f>
         <v>3</v>
       </c>
-      <c r="V5" t="str">
+      <c r="Z5">
+        <v>10</v>
+      </c>
+      <c r="AA5" t="str">
         <f t="shared" si="3"/>
         <v>GPB2</v>
       </c>
-      <c r="W5" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y5">
+      <c r="AB5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD5">
         <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AE5">
+        <v>5</v>
+      </c>
+      <c r="AF5" t="s">
         <v>72</v>
       </c>
-      <c r="AA5" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="AD5">
-        <f t="shared" ref="AD5:AD16" si="11">AD4+1</f>
+      <c r="AG5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AL5">
+        <f t="shared" ref="AL5:AL16" si="11">AL4+1</f>
         <v>3</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AM5">
+        <v>10</v>
+      </c>
+      <c r="AN5" t="str">
         <f t="shared" si="5"/>
         <v>GPB2</v>
       </c>
-      <c r="AF5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH5">
+      <c r="AO5" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP5">
+        <v>5</v>
+      </c>
+      <c r="AQ5">
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AS5" t="s">
         <v>72</v>
       </c>
-      <c r="AJ5" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT5" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="7"/>
         <v>7</v>
@@ -1545,68 +1731,86 @@
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="M6" t="str">
+      <c r="M6">
+        <v>11</v>
+      </c>
+      <c r="N6" t="str">
         <f t="shared" si="0"/>
         <v>GPB3</v>
       </c>
-      <c r="N6" s="5" t="str">
+      <c r="O6" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 4 Positive Out</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
         <v>73</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="T6" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="V6" t="str">
+      <c r="Z6">
+        <v>11</v>
+      </c>
+      <c r="AA6" t="str">
         <f t="shared" si="3"/>
         <v>GPB3</v>
       </c>
-      <c r="W6" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y6">
+      <c r="AB6" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD6">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AE6">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="s">
         <v>73</v>
       </c>
-      <c r="AA6" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD6">
+      <c r="AG6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL6">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="AE6" t="str">
+      <c r="AM6">
+        <v>11</v>
+      </c>
+      <c r="AN6" t="str">
         <f t="shared" si="5"/>
         <v>GPB3</v>
       </c>
-      <c r="AF6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH6">
+      <c r="AO6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP6">
+        <v>4</v>
+      </c>
+      <c r="AQ6">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AS6" t="s">
         <v>73</v>
       </c>
-      <c r="AJ6" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT6" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="7"/>
         <v>9</v>
@@ -1637,68 +1841,86 @@
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="M7" t="str">
+      <c r="M7">
+        <v>12</v>
+      </c>
+      <c r="N7" t="str">
         <f t="shared" si="0"/>
         <v>GPB4</v>
       </c>
-      <c r="N7" s="5" t="str">
+      <c r="O7" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 5 Positive Out</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="T7" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="U7">
+      <c r="Y7">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="V7" t="str">
+      <c r="Z7">
+        <v>12</v>
+      </c>
+      <c r="AA7" t="str">
         <f t="shared" si="3"/>
         <v>GPB4</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y7">
+      <c r="AB7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD7">
         <f t="shared" si="4"/>
         <v>24</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AE7">
+        <v>3</v>
+      </c>
+      <c r="AF7" t="s">
         <v>74</v>
       </c>
-      <c r="AA7" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="AD7">
+      <c r="AG7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL7">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="AE7" t="str">
+      <c r="AM7">
+        <v>12</v>
+      </c>
+      <c r="AN7" t="str">
         <f t="shared" si="5"/>
         <v>GPB4</v>
       </c>
-      <c r="AF7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AH7">
+      <c r="AO7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AP7">
+        <v>3</v>
+      </c>
+      <c r="AQ7">
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AS7" t="s">
         <v>74</v>
       </c>
-      <c r="AJ7" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT7" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="7"/>
         <v>11</v>
@@ -1723,71 +1945,89 @@
         <v>59</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L8">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="M8" t="str">
+      <c r="M8">
+        <v>13</v>
+      </c>
+      <c r="N8" t="str">
         <f t="shared" si="0"/>
         <v>GPB5</v>
       </c>
-      <c r="N8" s="5" t="str">
+      <c r="O8" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 6 Positive Out</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8" t="s">
         <v>75</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="T8" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="U8">
+      <c r="Y8">
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="V8" t="str">
+      <c r="Z8">
+        <v>13</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="3"/>
         <v>GPB5</v>
       </c>
-      <c r="W8" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y8">
+      <c r="AB8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD8">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AE8">
+        <v>2</v>
+      </c>
+      <c r="AF8" t="s">
         <v>75</v>
       </c>
-      <c r="AA8" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="AD8">
+      <c r="AG8" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="AL8">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="AE8" t="str">
+      <c r="AM8">
+        <v>13</v>
+      </c>
+      <c r="AN8" t="str">
         <f t="shared" si="5"/>
         <v>GPB5</v>
       </c>
-      <c r="AH8">
+      <c r="AP8">
+        <v>2</v>
+      </c>
+      <c r="AQ8">
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="AI8" t="s">
+      <c r="AS8" t="s">
         <v>75</v>
       </c>
-      <c r="AJ8" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT8" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="7"/>
         <v>13</v>
@@ -1818,65 +2058,83 @@
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="M9" t="str">
+      <c r="M9">
+        <v>14</v>
+      </c>
+      <c r="N9" t="str">
         <f t="shared" si="0"/>
         <v>GPB6</v>
       </c>
-      <c r="N9" s="5" t="str">
+      <c r="O9" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 7 Positive Out</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
         <v>76</v>
       </c>
-      <c r="R9" s="5" t="s">
+      <c r="T9" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="U9">
+      <c r="Y9">
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="V9" t="str">
+      <c r="Z9">
+        <v>14</v>
+      </c>
+      <c r="AA9" t="str">
         <f t="shared" si="3"/>
         <v>GPB6</v>
       </c>
-      <c r="W9" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y9">
+      <c r="AB9" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD9">
         <f t="shared" si="4"/>
         <v>22</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AE9">
+        <v>1</v>
+      </c>
+      <c r="AF9" t="s">
         <v>76</v>
       </c>
-      <c r="AA9" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD9">
+      <c r="AG9" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL9">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="AE9" t="str">
+      <c r="AM9">
+        <v>14</v>
+      </c>
+      <c r="AN9" t="str">
         <f t="shared" si="5"/>
         <v>GPB6</v>
       </c>
-      <c r="AH9">
+      <c r="AP9">
+        <v>1</v>
+      </c>
+      <c r="AQ9">
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="AI9" t="s">
+      <c r="AS9" t="s">
         <v>76</v>
       </c>
-      <c r="AJ9" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT9" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="7"/>
         <v>15</v>
@@ -1901,68 +2159,86 @@
         <v>60</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L10">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="M10" t="str">
+      <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10" t="str">
         <f t="shared" si="0"/>
         <v>GPB7</v>
       </c>
-      <c r="N10" s="5" t="str">
+      <c r="O10" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Valve 8 Positive Out</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" t="s">
         <v>77</v>
       </c>
-      <c r="U10">
+      <c r="Y10">
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="V10" t="str">
+      <c r="Z10">
+        <v>15</v>
+      </c>
+      <c r="AA10" t="str">
         <f t="shared" si="3"/>
         <v>GPB7</v>
       </c>
-      <c r="W10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y10">
+      <c r="AB10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD10">
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10" t="s">
         <v>77</v>
       </c>
-      <c r="AA10" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="AD10">
+      <c r="AG10" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL10">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="AE10" t="str">
+      <c r="AM10">
+        <v>15</v>
+      </c>
+      <c r="AN10" t="str">
         <f t="shared" si="5"/>
         <v>GPB7</v>
       </c>
-      <c r="AH10">
+      <c r="AP10">
+        <v>0</v>
+      </c>
+      <c r="AQ10">
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AS10" t="s">
         <v>77</v>
       </c>
-      <c r="AJ10" s="5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT10" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="7"/>
         <v>17</v>
@@ -1987,82 +2263,82 @@
         <v>61</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L11">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>78</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>81</v>
       </c>
-      <c r="S11" t="s">
-        <v>164</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="U11">
+      <c r="U11" t="s">
+        <v>162</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y11">
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
-      <c r="V11" t="s">
+      <c r="AA11" t="s">
         <v>78</v>
       </c>
-      <c r="W11" s="5" t="s">
+      <c r="AB11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Y11">
+      <c r="AD11">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AF11" t="s">
         <v>81</v>
       </c>
-      <c r="AA11" s="5" t="s">
+      <c r="AG11" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="AH11" t="s">
         <v>162</v>
       </c>
-      <c r="AB11" t="s">
-        <v>164</v>
-      </c>
-      <c r="AC11" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD11">
+      <c r="AK11" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AL11">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AN11" t="s">
         <v>78</v>
       </c>
-      <c r="AF11" s="5" t="s">
+      <c r="AO11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AH11">
+      <c r="AQ11">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AS11" t="s">
         <v>81</v>
       </c>
-      <c r="AJ11" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT11" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="7"/>
         <v>19</v>
@@ -2090,76 +2366,76 @@
         <v>15</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L12">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>79</v>
       </c>
-      <c r="N12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P12">
+      <c r="O12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>82</v>
       </c>
-      <c r="S12" t="s">
-        <v>165</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="U12">
+      <c r="U12" t="s">
+        <v>163</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="V12" t="s">
+      <c r="AA12" t="s">
         <v>79</v>
       </c>
-      <c r="W12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y12">
+      <c r="AB12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD12">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="Z12" t="s">
+      <c r="AF12" t="s">
         <v>82</v>
       </c>
-      <c r="AB12" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC12" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AD12">
+      <c r="AH12" t="s">
+        <v>163</v>
+      </c>
+      <c r="AK12" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL12">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AN12" t="s">
         <v>79</v>
       </c>
-      <c r="AF12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH12">
+      <c r="AO12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ12">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="AI12" t="s">
+      <c r="AS12" t="s">
         <v>82</v>
       </c>
-      <c r="AL12" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AV12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="7"/>
         <v>21</v>
@@ -2184,79 +2460,79 @@
         <v>62</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L13">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>80</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="S13" t="s">
         <v>83</v>
       </c>
-      <c r="R13" s="5" t="s">
+      <c r="T13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S13" t="s">
-        <v>166</v>
-      </c>
-      <c r="T13" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="U13">
+      <c r="U13" t="s">
+        <v>164</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y13">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="V13" t="s">
+      <c r="AA13" t="s">
         <v>80</v>
       </c>
-      <c r="Y13">
+      <c r="AD13">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="Z13" t="s">
+      <c r="AF13" t="s">
         <v>83</v>
       </c>
-      <c r="AA13" s="5" t="s">
+      <c r="AG13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" t="s">
-        <v>166</v>
-      </c>
-      <c r="AC13" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD13">
+      <c r="AH13" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL13">
         <f t="shared" si="11"/>
         <v>11</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AN13" t="s">
         <v>80</v>
       </c>
-      <c r="AH13">
+      <c r="AQ13">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AS13" t="s">
         <v>83</v>
       </c>
-      <c r="AJ13" s="5" t="s">
+      <c r="AT13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AL13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AV13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="7"/>
         <v>23</v>
@@ -2281,88 +2557,88 @@
         <v>63</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="L14">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>13</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>84</v>
       </c>
-      <c r="R14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S14" t="s">
-        <v>167</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="U14">
+      <c r="T14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" t="s">
+        <v>165</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y14">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="V14" t="s">
+      <c r="AA14" t="s">
         <v>13</v>
       </c>
-      <c r="W14" s="5" t="s">
+      <c r="AB14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Y14">
+      <c r="AD14">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AF14" t="s">
         <v>84</v>
       </c>
-      <c r="AA14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>167</v>
-      </c>
-      <c r="AC14" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="AD14">
+      <c r="AG14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="AL14">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AN14" t="s">
         <v>13</v>
       </c>
-      <c r="AF14" s="5" t="s">
+      <c r="AO14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AH14">
+      <c r="AQ14">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="AI14" t="s">
+      <c r="AS14" t="s">
         <v>84</v>
       </c>
-      <c r="AJ14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="7"/>
         <v>25</v>
@@ -2387,88 +2663,88 @@
         <v>64</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L15">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="O15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>85</v>
       </c>
-      <c r="R15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S15" t="s">
-        <v>142</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="U15">
+      <c r="T15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15" t="s">
+        <v>141</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y15">
         <f t="shared" si="10"/>
         <v>13</v>
       </c>
-      <c r="V15" t="s">
+      <c r="AA15" t="s">
         <v>12</v>
       </c>
-      <c r="W15" s="5" t="s">
+      <c r="AB15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Y15">
+      <c r="AD15">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="Z15" t="s">
+      <c r="AF15" t="s">
         <v>85</v>
       </c>
-      <c r="AA15" s="5" t="s">
+      <c r="AG15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AB15" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD15">
+      <c r="AH15" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK15" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL15">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="AE15" t="s">
+      <c r="AN15" t="s">
         <v>12</v>
       </c>
-      <c r="AF15" s="5" t="s">
+      <c r="AO15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AH15">
+      <c r="AQ15">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AS15" t="s">
         <v>85</v>
       </c>
-      <c r="AJ15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AL15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AT15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="7"/>
         <v>27</v>
@@ -2490,70 +2766,70 @@
         <v>51</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L16">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>80</v>
       </c>
-      <c r="P16">
-        <v>15</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="Q16">
+        <v>15</v>
+      </c>
+      <c r="S16" t="s">
         <v>86</v>
       </c>
-      <c r="R16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="S16" t="s">
-        <v>168</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="U16">
+      <c r="T16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" t="s">
+        <v>166</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y16">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="V16" t="s">
+      <c r="AA16" t="s">
         <v>80</v>
       </c>
-      <c r="Y16">
-        <v>15</v>
-      </c>
-      <c r="Z16" t="s">
+      <c r="AD16">
+        <v>15</v>
+      </c>
+      <c r="AF16" t="s">
         <v>86</v>
       </c>
-      <c r="AA16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB16" t="s">
-        <v>168</v>
-      </c>
-      <c r="AC16" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AD16">
+      <c r="AG16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>166</v>
+      </c>
+      <c r="AK16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL16">
         <f t="shared" si="11"/>
         <v>14</v>
       </c>
-      <c r="AE16" t="s">
+      <c r="AN16" t="s">
         <v>80</v>
       </c>
-      <c r="AH16">
-        <v>15</v>
-      </c>
-      <c r="AI16" t="s">
+      <c r="AQ16">
+        <v>15</v>
+      </c>
+      <c r="AS16" t="s">
         <v>86</v>
       </c>
-      <c r="AJ16" s="5" t="s">
+      <c r="AT16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AL16" t="s">
-        <v>168</v>
+      <c r="AV16" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2609,7 +2885,7 @@
         <v>65</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,7 +2900,7 @@
         <v>54</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F19">
         <f t="shared" si="8"/>
@@ -2652,7 +2928,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F20">
         <f t="shared" si="8"/>
@@ -2665,7 +2941,7 @@
         <v>66</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2693,7 +2969,7 @@
         <v>67</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2721,7 +2997,12 @@
         <v>68</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2735,18 +3016,18 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="A8:H12"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -2790,27 +3071,27 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>140</v>
+      </c>
+      <c r="M1" t="s">
         <v>141</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>142</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>143</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>144</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>145</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2825,13 +3106,13 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
         <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2846,7 +3127,7 @@
         <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2861,10 +3142,10 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2876,4 +3157,208 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates pin layout for fourth MCP23017
</commit_message>
<xml_diff>
--- a/Design diagrams/Relay and Pin Layout.xlsx
+++ b/Design diagrams/Relay and Pin Layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18855" windowHeight="6135" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18855" windowHeight="6135" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Relays" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="SPI Addresses" sheetId="3" r:id="rId3"/>
     <sheet name="XLR Mapping" sheetId="4" r:id="rId4"/>
     <sheet name="RTD Pins" sheetId="5" r:id="rId5"/>
+    <sheet name="ADC Channels" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="205">
   <si>
     <t>Relay</t>
   </si>
@@ -324,12 +325,6 @@
     <t>Alarm Switch In</t>
   </si>
   <si>
-    <t>Heat Out 1</t>
-  </si>
-  <si>
-    <t>Heat Out 2</t>
-  </si>
-  <si>
     <t>Wort Pump Out</t>
   </si>
   <si>
@@ -585,12 +580,6 @@
     <t>csPin</t>
   </si>
   <si>
-    <t>misoPin</t>
-  </si>
-  <si>
-    <t>mosiPin</t>
-  </si>
-  <si>
     <t>clkPin</t>
   </si>
   <si>
@@ -603,9 +592,6 @@
     <t>BLK</t>
   </si>
   <si>
-    <t>0x21</t>
-  </si>
-  <si>
     <t>Temp 2 CS (HLT)</t>
   </si>
   <si>
@@ -622,13 +608,49 @@
   </si>
   <si>
     <t>TEST123</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Kettle</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>MCP23017-2 (0x22)</t>
+  </si>
+  <si>
+    <t>Heat Relay Out 1</t>
+  </si>
+  <si>
+    <t>Heat Relay Out 2</t>
+  </si>
+  <si>
+    <t>MCP23017-4 (0x23)</t>
+  </si>
+  <si>
+    <t>MCP23017-1 (0x20)</t>
+  </si>
+  <si>
+    <t>0x23</t>
+  </si>
+  <si>
+    <t>MCP23017-4</t>
+  </si>
+  <si>
+    <t>misoPin / SDO</t>
+  </si>
+  <si>
+    <t>mosiPin / SDI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,6 +660,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -665,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -680,7 +711,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -964,7 +997,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1002,14 +1035,14 @@
         <v>1</v>
       </c>
       <c r="B3" t="str">
-        <f>"Valve "&amp;A3&amp;" Positive"</f>
-        <v>Valve 1 Positive</v>
+        <f>"Valve "&amp;A10&amp;" Positive"</f>
+        <v>Valve 8 Positive</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,140 +1051,140 @@
         <v>2</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" ref="B4:B10" si="0">"Valve "&amp;A4&amp;" Positive"</f>
-        <v>Valve 2 Positive</v>
+        <f>"Valve "&amp;A9&amp;" Positive"</f>
+        <v>Valve 7 Positive</v>
       </c>
       <c r="D4">
         <f>D3+1</f>
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A18" si="1">A4+1</f>
+        <f t="shared" ref="A5:A18" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 3 Positive</v>
+        <f>"Valve "&amp;A8&amp;" Positive"</f>
+        <v>Valve 6 Positive</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:D10" si="2">D4+1</f>
+        <f t="shared" ref="D5:D10" si="1">D4+1</f>
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <f>"Valve "&amp;A7&amp;" Positive"</f>
+        <v>Valve 5 Positive</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 4 Positive</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
       <c r="E6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f>"Valve "&amp;A6&amp;" Positive"</f>
+        <v>Valve 4 Positive</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 5 Positive</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"Valve "&amp;A5&amp;" Positive"</f>
+        <v>Valve 3 Positive</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 6 Positive</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"Valve "&amp;A4&amp;" Positive"</f>
+        <v>Valve 2 Positive</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 7 Positive</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"Valve "&amp;A3&amp;" Positive"</f>
+        <v>Valve 1 Positive</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>Valve 8 Positive</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1160,7 +1193,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1169,7 +1202,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B17" t="str">
@@ -1179,7 +1212,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B18" t="str">
@@ -1195,25 +1228,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AV25"/>
+  <dimension ref="A1:BF25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1226,7 +1263,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" s="2" t="s">
-        <v>69</v>
+        <v>200</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1237,7 +1274,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="Y1" s="2" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -1248,7 +1285,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
       <c r="AL1" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="AM1" s="2"/>
       <c r="AN1" s="2"/>
@@ -1257,9 +1294,18 @@
       <c r="AQ1" s="2"/>
       <c r="AR1" s="2"/>
       <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="2"/>
+      <c r="BD1" s="2"/>
+      <c r="BE1" s="2"/>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1285,13 +1331,13 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="L2" t="s">
         <v>7</v>
       </c>
       <c r="M2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N2" t="s">
         <v>8</v>
@@ -1303,7 +1349,7 @@
         <v>7</v>
       </c>
       <c r="R2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="S2" t="s">
         <v>8</v>
@@ -1312,16 +1358,16 @@
         <v>9</v>
       </c>
       <c r="U2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="X2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="Y2" t="s">
         <v>7</v>
       </c>
       <c r="Z2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AA2" t="s">
         <v>8</v>
@@ -1333,7 +1379,7 @@
         <v>7</v>
       </c>
       <c r="AE2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AF2" t="s">
         <v>8</v>
@@ -1342,16 +1388,16 @@
         <v>9</v>
       </c>
       <c r="AH2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AK2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AL2" t="s">
         <v>7</v>
       </c>
       <c r="AM2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AN2" t="s">
         <v>8</v>
@@ -1360,22 +1406,52 @@
         <v>9</v>
       </c>
       <c r="AP2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="AQ2" t="s">
         <v>7</v>
       </c>
+      <c r="AR2" t="s">
+        <v>8</v>
+      </c>
       <c r="AS2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>189</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>8</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="BA2" t="s">
         <v>9</v>
       </c>
-      <c r="AV2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="BB2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>7</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>8</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1385,7 +1461,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F3">
@@ -1397,7 +1473,7 @@
       <c r="H3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L3">
@@ -1410,7 +1486,7 @@
         <f>"GPB"&amp;L3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="O3" s="5" t="str">
+      <c r="O3" s="7" t="str">
         <f>"Valve "&amp;L3&amp;" Positive Out"</f>
         <v>Valve 1 Positive Out</v>
       </c>
@@ -1424,8 +1500,8 @@
       <c r="S3" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>104</v>
+      <c r="T3" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="Y3">
         <v>1</v>
@@ -1437,8 +1513,8 @@
         <f>"GPB"&amp;Y3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="AB3" s="5" t="s">
-        <v>111</v>
+      <c r="AB3" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="AD3">
         <f>AD4+1</f>
@@ -1450,8 +1526,8 @@
       <c r="AF3" t="s">
         <v>70</v>
       </c>
-      <c r="AG3" s="5" t="s">
-        <v>119</v>
+      <c r="AG3" s="7" t="s">
+        <v>117</v>
       </c>
       <c r="AL3">
         <v>1</v>
@@ -1463,8 +1539,8 @@
         <f>"GPB"&amp;AL3-1</f>
         <v>GPB0</v>
       </c>
-      <c r="AO3" s="5" t="s">
-        <v>109</v>
+      <c r="AO3" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="AP3">
         <v>7</v>
@@ -1473,14 +1549,40 @@
         <f>AQ4+1</f>
         <v>28</v>
       </c>
-      <c r="AS3" t="s">
+      <c r="AR3" t="s">
         <v>70</v>
       </c>
-      <c r="AT3" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS3" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3">
+        <v>8</v>
+      </c>
+      <c r="AZ3" t="str">
+        <f>"GPB"&amp;AX3-1</f>
+        <v>GPB0</v>
+      </c>
+      <c r="BA3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB3">
+        <v>7</v>
+      </c>
+      <c r="BC3">
+        <f>BC4+1</f>
+        <v>28</v>
+      </c>
+      <c r="BD3" t="s">
+        <v>70</v>
+      </c>
+      <c r="BE3" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+2</f>
         <v>3</v>
@@ -1491,7 +1593,7 @@
       <c r="C4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F4">
@@ -1504,7 +1606,7 @@
       <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="L4">
@@ -1518,7 +1620,7 @@
         <f t="shared" ref="N4:N10" si="0">"GPB"&amp;L4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="O4" s="5" t="str">
+      <c r="O4" s="7" t="str">
         <f t="shared" ref="O4:O10" si="1">"Valve "&amp;L4&amp;" Positive Out"</f>
         <v>Valve 2 Positive Out</v>
       </c>
@@ -1532,8 +1634,8 @@
       <c r="S4" t="s">
         <v>71</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>105</v>
+      <c r="T4" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="Y4">
         <f>Y3+1</f>
@@ -1546,8 +1648,8 @@
         <f t="shared" ref="AA4:AA10" si="3">"GPB"&amp;Y4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="AB4" s="5" t="s">
-        <v>113</v>
+      <c r="AB4" s="7" t="s">
+        <v>111</v>
       </c>
       <c r="AD4">
         <f t="shared" ref="AD4:AD15" si="4">AD5+1</f>
@@ -1559,8 +1661,8 @@
       <c r="AF4" t="s">
         <v>71</v>
       </c>
-      <c r="AG4" s="5" t="s">
-        <v>120</v>
+      <c r="AG4" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="AL4">
         <f>AL3+1</f>
@@ -1573,8 +1675,8 @@
         <f t="shared" ref="AN4:AN10" si="5">"GPB"&amp;AL4-1</f>
         <v>GPB1</v>
       </c>
-      <c r="AO4" s="5" t="s">
-        <v>108</v>
+      <c r="AO4" s="7" t="s">
+        <v>106</v>
       </c>
       <c r="AP4">
         <v>6</v>
@@ -1583,16 +1685,43 @@
         <f t="shared" ref="AQ4:AQ15" si="6">AQ5+1</f>
         <v>27</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="AR4" t="s">
         <v>71</v>
       </c>
-      <c r="AT4" s="5" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="AX4">
+        <f>AX3+1</f>
+        <v>2</v>
+      </c>
+      <c r="AY4">
+        <v>9</v>
+      </c>
+      <c r="AZ4" t="str">
+        <f t="shared" ref="AZ4:AZ10" si="7">"GPB"&amp;AX4-1</f>
+        <v>GPB1</v>
+      </c>
+      <c r="BA4" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="BB4">
+        <v>6</v>
+      </c>
+      <c r="BC4">
+        <f t="shared" ref="BC4:BC15" si="8">BC5+1</f>
+        <v>27</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BE4" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" ref="A5:A22" si="7">A4+2</f>
+        <f t="shared" ref="A5:A22" si="9">A4+2</f>
         <v>5</v>
       </c>
       <c r="B5" t="s">
@@ -1601,11 +1730,11 @@
       <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F22" si="8">F4+2</f>
+        <f t="shared" ref="F5:F22" si="10">F4+2</f>
         <v>6</v>
       </c>
       <c r="G5" t="s">
@@ -1614,11 +1743,11 @@
       <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L16" si="9">L4+1</f>
+        <f t="shared" ref="L5:L16" si="11">L4+1</f>
         <v>3</v>
       </c>
       <c r="M5">
@@ -1628,7 +1757,7 @@
         <f t="shared" si="0"/>
         <v>GPB2</v>
       </c>
-      <c r="O5" s="5" t="str">
+      <c r="O5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 3 Positive Out</v>
       </c>
@@ -1642,11 +1771,11 @@
       <c r="S5" t="s">
         <v>72</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>103</v>
+      <c r="T5" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="Y5">
-        <f t="shared" ref="Y5:Y16" si="10">Y4+1</f>
+        <f t="shared" ref="Y5:Y16" si="12">Y4+1</f>
         <v>3</v>
       </c>
       <c r="Z5">
@@ -1656,8 +1785,8 @@
         <f t="shared" si="3"/>
         <v>GPB2</v>
       </c>
-      <c r="AB5" s="5" t="s">
-        <v>114</v>
+      <c r="AB5" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="AD5">
         <f t="shared" si="4"/>
@@ -1669,11 +1798,11 @@
       <c r="AF5" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" s="5" t="s">
-        <v>121</v>
+      <c r="AG5" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="AL5">
-        <f t="shared" ref="AL5:AL16" si="11">AL4+1</f>
+        <f t="shared" ref="AL5:AL16" si="13">AL4+1</f>
         <v>3</v>
       </c>
       <c r="AM5">
@@ -1683,8 +1812,8 @@
         <f t="shared" si="5"/>
         <v>GPB2</v>
       </c>
-      <c r="AO5" s="5" t="s">
-        <v>193</v>
+      <c r="AO5" s="7" t="s">
+        <v>188</v>
       </c>
       <c r="AP5">
         <v>5</v>
@@ -1693,16 +1822,43 @@
         <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AR5" t="s">
         <v>72</v>
       </c>
-      <c r="AT5" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS5" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="AX5">
+        <f t="shared" ref="AX5:AX16" si="14">AX4+1</f>
+        <v>3</v>
+      </c>
+      <c r="AY5">
+        <v>10</v>
+      </c>
+      <c r="AZ5" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB2</v>
+      </c>
+      <c r="BA5" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="BB5">
+        <v>5</v>
+      </c>
+      <c r="BC5">
+        <f t="shared" si="8"/>
+        <v>26</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>72</v>
+      </c>
+      <c r="BE5" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -1711,11 +1867,11 @@
       <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="7" t="s">
         <v>94</v>
       </c>
       <c r="F6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="G6" t="s">
@@ -1724,11 +1880,11 @@
       <c r="H6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>98</v>
+      <c r="I6" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="L6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>4</v>
       </c>
       <c r="M6">
@@ -1738,7 +1894,7 @@
         <f t="shared" si="0"/>
         <v>GPB3</v>
       </c>
-      <c r="O6" s="5" t="str">
+      <c r="O6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 4 Positive Out</v>
       </c>
@@ -1752,11 +1908,11 @@
       <c r="S6" t="s">
         <v>73</v>
       </c>
-      <c r="T6" s="6" t="s">
-        <v>106</v>
+      <c r="T6" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="Z6">
@@ -1766,8 +1922,8 @@
         <f t="shared" si="3"/>
         <v>GPB3</v>
       </c>
-      <c r="AB6" s="5" t="s">
-        <v>112</v>
+      <c r="AB6" s="7" t="s">
+        <v>110</v>
       </c>
       <c r="AD6">
         <f t="shared" si="4"/>
@@ -1779,11 +1935,11 @@
       <c r="AF6" t="s">
         <v>73</v>
       </c>
-      <c r="AG6" s="5" t="s">
-        <v>122</v>
+      <c r="AG6" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="AL6">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>4</v>
       </c>
       <c r="AM6">
@@ -1793,8 +1949,8 @@
         <f t="shared" si="5"/>
         <v>GPB3</v>
       </c>
-      <c r="AO6" s="5" t="s">
-        <v>107</v>
+      <c r="AO6" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="AP6">
         <v>4</v>
@@ -1803,16 +1959,43 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AR6" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS6" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="AX6">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="AY6">
+        <v>11</v>
+      </c>
+      <c r="AZ6" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB3</v>
+      </c>
+      <c r="BA6" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="BB6">
+        <v>4</v>
+      </c>
+      <c r="BC6">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="BD6" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE6" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="B7" t="s">
@@ -1821,11 +2004,11 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="G7" t="s">
@@ -1834,11 +2017,11 @@
       <c r="H7" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>99</v>
+      <c r="I7" s="7" t="s">
+        <v>198</v>
       </c>
       <c r="L7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="M7">
@@ -1848,7 +2031,7 @@
         <f t="shared" si="0"/>
         <v>GPB4</v>
       </c>
-      <c r="O7" s="5" t="str">
+      <c r="O7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 5 Positive Out</v>
       </c>
@@ -1862,11 +2045,11 @@
       <c r="S7" t="s">
         <v>74</v>
       </c>
-      <c r="T7" s="5" t="s">
-        <v>100</v>
+      <c r="T7" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="Z7">
@@ -1876,8 +2059,8 @@
         <f t="shared" si="3"/>
         <v>GPB4</v>
       </c>
-      <c r="AB7" s="5" t="s">
-        <v>115</v>
+      <c r="AB7" s="7" t="s">
+        <v>113</v>
       </c>
       <c r="AD7">
         <f t="shared" si="4"/>
@@ -1889,11 +2072,11 @@
       <c r="AF7" t="s">
         <v>74</v>
       </c>
-      <c r="AG7" s="5" t="s">
-        <v>123</v>
+      <c r="AG7" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5</v>
       </c>
       <c r="AM7">
@@ -1903,8 +2086,8 @@
         <f t="shared" si="5"/>
         <v>GPB4</v>
       </c>
-      <c r="AO7" s="5" t="s">
-        <v>156</v>
+      <c r="AO7" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="AP7">
         <v>3</v>
@@ -1913,16 +2096,38 @@
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AR7" t="s">
         <v>74</v>
       </c>
-      <c r="AT7" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX7">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="AY7">
+        <v>12</v>
+      </c>
+      <c r="AZ7" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB4</v>
+      </c>
+      <c r="BA7" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="BB7">
+        <v>3</v>
+      </c>
+      <c r="BC7">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>74</v>
+      </c>
+      <c r="BE7" s="7"/>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -1931,11 +2136,11 @@
       <c r="C8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
       <c r="G8" t="s">
@@ -1944,11 +2149,11 @@
       <c r="H8" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>149</v>
+      <c r="I8" s="7" t="s">
+        <v>147</v>
       </c>
       <c r="L8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="M8">
@@ -1958,7 +2163,7 @@
         <f t="shared" si="0"/>
         <v>GPB5</v>
       </c>
-      <c r="O8" s="5" t="str">
+      <c r="O8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 6 Positive Out</v>
       </c>
@@ -1972,11 +2177,11 @@
       <c r="S8" t="s">
         <v>75</v>
       </c>
-      <c r="T8" s="5" t="s">
-        <v>101</v>
+      <c r="T8" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="Z8">
@@ -1986,8 +2191,8 @@
         <f t="shared" si="3"/>
         <v>GPB5</v>
       </c>
-      <c r="AB8" s="5" t="s">
-        <v>116</v>
+      <c r="AB8" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="AD8">
         <f t="shared" si="4"/>
@@ -1999,11 +2204,11 @@
       <c r="AF8" t="s">
         <v>75</v>
       </c>
-      <c r="AG8" s="5" t="s">
-        <v>124</v>
+      <c r="AG8" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="AL8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6</v>
       </c>
       <c r="AM8">
@@ -2020,16 +2225,35 @@
         <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="AS8" t="s">
+      <c r="AR8" t="s">
         <v>75</v>
       </c>
-      <c r="AT8" s="5" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="9" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX8">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="AY8">
+        <v>13</v>
+      </c>
+      <c r="AZ8" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB5</v>
+      </c>
+      <c r="BB8">
+        <v>2</v>
+      </c>
+      <c r="BC8">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>75</v>
+      </c>
+      <c r="BE8" s="7"/>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="B9" t="s">
@@ -2038,11 +2262,11 @@
       <c r="C9" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="7" t="s">
         <v>88</v>
       </c>
       <c r="F9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14</v>
       </c>
       <c r="G9" t="s">
@@ -2051,11 +2275,11 @@
       <c r="H9" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="L9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="M9">
@@ -2065,7 +2289,7 @@
         <f t="shared" si="0"/>
         <v>GPB6</v>
       </c>
-      <c r="O9" s="5" t="str">
+      <c r="O9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 7 Positive Out</v>
       </c>
@@ -2079,11 +2303,11 @@
       <c r="S9" t="s">
         <v>76</v>
       </c>
-      <c r="T9" s="5" t="s">
-        <v>102</v>
+      <c r="T9" s="7" t="s">
+        <v>100</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="Z9">
@@ -2093,8 +2317,8 @@
         <f t="shared" si="3"/>
         <v>GPB6</v>
       </c>
-      <c r="AB9" s="5" t="s">
-        <v>117</v>
+      <c r="AB9" s="7" t="s">
+        <v>115</v>
       </c>
       <c r="AD9">
         <f t="shared" si="4"/>
@@ -2106,11 +2330,11 @@
       <c r="AF9" t="s">
         <v>76</v>
       </c>
-      <c r="AG9" s="5" t="s">
-        <v>125</v>
+      <c r="AG9" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7</v>
       </c>
       <c r="AM9">
@@ -2127,16 +2351,35 @@
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="AS9" t="s">
+      <c r="AR9" t="s">
         <v>76</v>
       </c>
-      <c r="AT9" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX9">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="AY9">
+        <v>14</v>
+      </c>
+      <c r="AZ9" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB6</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
+      <c r="BC9">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>76</v>
+      </c>
+      <c r="BE9" s="7"/>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="B10" t="s">
@@ -2145,11 +2388,11 @@
       <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="7" t="s">
         <v>89</v>
       </c>
       <c r="F10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="G10" t="s">
@@ -2158,11 +2401,11 @@
       <c r="H10" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>148</v>
+      <c r="I10" s="7" t="s">
+        <v>146</v>
       </c>
       <c r="L10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="M10">
@@ -2172,7 +2415,7 @@
         <f t="shared" si="0"/>
         <v>GPB7</v>
       </c>
-      <c r="O10" s="5" t="str">
+      <c r="O10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Valve 8 Positive Out</v>
       </c>
@@ -2187,7 +2430,7 @@
         <v>77</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="Z10">
@@ -2197,8 +2440,8 @@
         <f t="shared" si="3"/>
         <v>GPB7</v>
       </c>
-      <c r="AB10" s="5" t="s">
-        <v>118</v>
+      <c r="AB10" s="7" t="s">
+        <v>116</v>
       </c>
       <c r="AD10">
         <f t="shared" si="4"/>
@@ -2210,11 +2453,11 @@
       <c r="AF10" t="s">
         <v>77</v>
       </c>
-      <c r="AG10" s="5" t="s">
-        <v>126</v>
+      <c r="AG10" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="AL10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="AM10">
@@ -2231,16 +2474,35 @@
         <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="AS10" t="s">
+      <c r="AR10" t="s">
         <v>77</v>
       </c>
-      <c r="AT10" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AX10">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="AY10">
+        <v>15</v>
+      </c>
+      <c r="AZ10" t="str">
+        <f t="shared" si="7"/>
+        <v>GPB7</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <f t="shared" si="8"/>
+        <v>21</v>
+      </c>
+      <c r="BD10" t="s">
+        <v>77</v>
+      </c>
+      <c r="BE10" s="7"/>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="B11" t="s">
@@ -2249,11 +2511,11 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="G11" t="s">
@@ -2263,16 +2525,16 @@
         <v>61</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="N11" t="s">
         <v>78</v>
       </c>
-      <c r="O11" s="5" t="s">
+      <c r="O11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="Q11">
@@ -2283,19 +2545,19 @@
         <v>81</v>
       </c>
       <c r="U11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="AA11" t="s">
         <v>78</v>
       </c>
-      <c r="AB11" s="5" t="s">
+      <c r="AB11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AD11">
@@ -2305,42 +2567,66 @@
       <c r="AF11" t="s">
         <v>81</v>
       </c>
-      <c r="AG11" s="5" t="s">
+      <c r="AG11" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH11" t="s">
         <v>160</v>
       </c>
-      <c r="AH11" t="s">
-        <v>162</v>
-      </c>
       <c r="AK11" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AL11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="AN11" t="s">
         <v>78</v>
       </c>
-      <c r="AO11" s="5" t="s">
+      <c r="AO11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AQ11">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AR11" t="s">
         <v>81</v>
       </c>
-      <c r="AT11" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS11" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>160</v>
+      </c>
+      <c r="AW11" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AX11">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BC11">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="BD11" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE11" s="7"/>
+      <c r="BF11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="B12" t="s">
@@ -2349,11 +2635,11 @@
       <c r="C12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="7" t="s">
         <v>90</v>
       </c>
       <c r="F12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
       <c r="G12" t="s">
@@ -2362,20 +2648,20 @@
       <c r="H12" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="N12" t="s">
         <v>79</v>
       </c>
-      <c r="O12" s="5" t="s">
+      <c r="O12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="Q12">
@@ -2386,19 +2672,19 @@
         <v>82</v>
       </c>
       <c r="U12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="X12" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="AA12" t="s">
         <v>79</v>
       </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AB12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="AD12">
@@ -2409,35 +2695,58 @@
         <v>82</v>
       </c>
       <c r="AH12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AK12" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AL12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>10</v>
       </c>
       <c r="AN12" t="s">
         <v>79</v>
       </c>
-      <c r="AO12" s="5" t="s">
+      <c r="AO12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="AQ12">
         <f t="shared" si="6"/>
         <v>19</v>
       </c>
-      <c r="AS12" t="s">
+      <c r="AR12" t="s">
         <v>82</v>
       </c>
-      <c r="AV12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AT12" t="s">
+        <v>161</v>
+      </c>
+      <c r="AW12" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AX12">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="AZ12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BA12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC12">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="BD12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BF12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="B13" t="s">
@@ -2446,11 +2755,11 @@
       <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="7" t="s">
         <v>91</v>
       </c>
       <c r="F13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22</v>
       </c>
       <c r="G13" t="s">
@@ -2460,13 +2769,13 @@
         <v>62</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="N13" t="s">
@@ -2479,17 +2788,17 @@
       <c r="S13" t="s">
         <v>83</v>
       </c>
-      <c r="T13" s="5" t="s">
+      <c r="T13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="U13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="AA13" t="s">
@@ -2502,17 +2811,17 @@
       <c r="AF13" t="s">
         <v>83</v>
       </c>
-      <c r="AG13" s="5" t="s">
+      <c r="AG13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AH13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AK13" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AL13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="AN13" t="s">
@@ -2522,19 +2831,42 @@
         <f t="shared" si="6"/>
         <v>18</v>
       </c>
-      <c r="AS13" t="s">
+      <c r="AR13" t="s">
         <v>83</v>
       </c>
-      <c r="AT13" s="5" t="s">
+      <c r="AS13" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AV13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AT13" t="s">
+        <v>162</v>
+      </c>
+      <c r="AW13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AX13">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="AZ13" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC13">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="BD13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="B14" t="s">
@@ -2543,11 +2875,11 @@
       <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
       <c r="G14" t="s">
@@ -2556,20 +2888,20 @@
       <c r="H14" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>131</v>
+      <c r="I14" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="L14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="N14" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="5" t="s">
+      <c r="O14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="Q14">
@@ -2579,23 +2911,23 @@
       <c r="S14" t="s">
         <v>84</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="T14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="U14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="AA14" t="s">
         <v>13</v>
       </c>
-      <c r="AB14" s="5" t="s">
+      <c r="AB14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="AD14">
@@ -2605,42 +2937,68 @@
       <c r="AF14" t="s">
         <v>84</v>
       </c>
-      <c r="AG14" s="5" t="s">
+      <c r="AG14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="AH14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AK14" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AL14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>12</v>
       </c>
       <c r="AN14" t="s">
         <v>13</v>
       </c>
-      <c r="AO14" s="5" t="s">
+      <c r="AO14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="AQ14">
         <f t="shared" si="6"/>
         <v>17</v>
       </c>
-      <c r="AS14" t="s">
+      <c r="AR14" t="s">
         <v>84</v>
       </c>
-      <c r="AT14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>163</v>
+      </c>
+      <c r="AW14" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AX14">
+        <f t="shared" si="14"/>
+        <v>12</v>
+      </c>
+      <c r="AZ14" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC14">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="BD14" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="BF14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="B15" t="s">
@@ -2649,11 +3007,11 @@
       <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="G15" t="s">
@@ -2662,20 +3020,20 @@
       <c r="H15" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>132</v>
+      <c r="I15" s="7" t="s">
+        <v>130</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="N15" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="5" t="s">
+      <c r="O15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q15">
@@ -2685,23 +3043,23 @@
       <c r="S15" t="s">
         <v>85</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="T15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="U15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>13</v>
       </c>
       <c r="AA15" t="s">
         <v>12</v>
       </c>
-      <c r="AB15" s="5" t="s">
+      <c r="AB15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AD15">
@@ -2711,42 +3069,68 @@
       <c r="AF15" t="s">
         <v>85</v>
       </c>
-      <c r="AG15" s="5" t="s">
+      <c r="AG15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="AH15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AK15" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AL15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13</v>
       </c>
       <c r="AN15" t="s">
         <v>12</v>
       </c>
-      <c r="AO15" s="5" t="s">
+      <c r="AO15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="AQ15">
         <f t="shared" si="6"/>
         <v>16</v>
       </c>
-      <c r="AS15" t="s">
+      <c r="AR15" t="s">
         <v>85</v>
       </c>
-      <c r="AT15" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:48" x14ac:dyDescent="0.25">
+      <c r="AS15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT15" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW15" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="AZ15" t="s">
+        <v>12</v>
+      </c>
+      <c r="BA15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC15">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="BD15" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="B16" t="s">
@@ -2756,7 +3140,7 @@
         <v>51</v>
       </c>
       <c r="F16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28</v>
       </c>
       <c r="G16" t="s">
@@ -2766,10 +3150,10 @@
         <v>51</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="N16" t="s">
@@ -2781,17 +3165,17 @@
       <c r="S16" t="s">
         <v>86</v>
       </c>
-      <c r="T16" s="5" t="s">
+      <c r="T16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="U16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="AA16" t="s">
@@ -2803,17 +3187,17 @@
       <c r="AF16" t="s">
         <v>86</v>
       </c>
-      <c r="AG16" s="5" t="s">
+      <c r="AG16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="AH16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AK16" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AL16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="AN16" t="s">
@@ -2822,19 +3206,41 @@
       <c r="AQ16">
         <v>15</v>
       </c>
-      <c r="AS16" t="s">
+      <c r="AR16" t="s">
         <v>86</v>
       </c>
-      <c r="AT16" s="5" t="s">
+      <c r="AS16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="AV16" t="s">
-        <v>166</v>
+      <c r="AT16" t="s">
+        <v>164</v>
+      </c>
+      <c r="AW16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" si="14"/>
+        <v>14</v>
+      </c>
+      <c r="AZ16" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC16">
+        <v>15</v>
+      </c>
+      <c r="BD16" t="s">
+        <v>86</v>
+      </c>
+      <c r="BE16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="BF16" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>29</v>
       </c>
       <c r="B17" t="s">
@@ -2843,11 +3249,11 @@
       <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>30</v>
       </c>
       <c r="G17" t="s">
@@ -2862,7 +3268,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>31</v>
       </c>
       <c r="B18" t="s">
@@ -2871,11 +3277,11 @@
       <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="7" t="s">
         <v>93</v>
       </c>
       <c r="F18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
       <c r="G18" t="s">
@@ -2884,13 +3290,13 @@
       <c r="H18" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>133</v>
+      <c r="I18" s="7" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>33</v>
       </c>
       <c r="B19" t="s">
@@ -2899,11 +3305,11 @@
       <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>154</v>
+      <c r="D19" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="F19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>34</v>
       </c>
       <c r="G19" t="s">
@@ -2912,13 +3318,13 @@
       <c r="H19" t="s">
         <v>15</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>35</v>
       </c>
       <c r="B20" t="s">
@@ -2927,11 +3333,11 @@
       <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>155</v>
+      <c r="D20" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="F20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
       <c r="G20" t="s">
@@ -2940,13 +3346,13 @@
       <c r="H20" t="s">
         <v>66</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>134</v>
+      <c r="I20" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>37</v>
       </c>
       <c r="B21" t="s">
@@ -2955,11 +3361,11 @@
       <c r="C21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>38</v>
       </c>
       <c r="G21" t="s">
@@ -2968,13 +3374,13 @@
       <c r="H21" t="s">
         <v>67</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>135</v>
+      <c r="I21" s="7" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="B22" t="s">
@@ -2983,11 +3389,11 @@
       <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="G22" t="s">
@@ -2996,13 +3402,13 @@
       <c r="H22" t="s">
         <v>68</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>136</v>
+      <c r="I22" s="7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3016,7 +3422,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,27 +3477,27 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" t="s">
         <v>140</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>141</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>142</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>143</v>
-      </c>
-      <c r="P1" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3109,10 +3515,13 @@
         <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3127,7 +3536,7 @@
         <v>40</v>
       </c>
       <c r="J6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -3142,10 +3551,10 @@
         <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -3164,7 +3573,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3177,22 +3586,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,19 +3609,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
         <v>174</v>
       </c>
-      <c r="D2" t="s">
-        <v>176</v>
-      </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3220,19 +3629,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>172</v>
       </c>
       <c r="F3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3240,19 +3649,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" t="s">
         <v>175</v>
       </c>
-      <c r="C4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D4" t="s">
-        <v>177</v>
-      </c>
       <c r="E4" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3265,7 +3674,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,38 +3684,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -3317,10 +3726,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>11</v>
@@ -3331,10 +3740,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -3345,10 +3754,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -3361,4 +3770,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Switches water and wort pump in pins to reflect how they are wired
</commit_message>
<xml_diff>
--- a/Design diagrams/Relay and Pin Layout.xlsx
+++ b/Design diagrams/Relay and Pin Layout.xlsx
@@ -20,6 +20,7 @@
     <sheet name="ADC Channels" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="204">
   <si>
     <t>Relay</t>
   </si>
@@ -605,9 +606,6 @@
   </si>
   <si>
     <t>MCP23017-3 (0x21)</t>
-  </si>
-  <si>
-    <t>TEST123</t>
   </si>
   <si>
     <t>Channel</t>
@@ -1228,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF25"/>
+  <dimension ref="A1:BF22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,7 +1261,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -1274,7 +1272,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="Y1" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
@@ -1295,7 +1293,7 @@
       <c r="AR1" s="2"/>
       <c r="AS1" s="2"/>
       <c r="AX1" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
@@ -1881,7 +1879,7 @@
         <v>57</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L6">
         <f t="shared" si="11"/>
@@ -2018,7 +2016,7 @@
         <v>58</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L7">
         <f t="shared" si="11"/>
@@ -2263,7 +2261,7 @@
         <v>46</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F9">
         <f t="shared" si="10"/>
@@ -2389,7 +2387,7 @@
         <v>47</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F10">
         <f t="shared" si="10"/>
@@ -2636,7 +2634,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12">
         <f t="shared" si="10"/>
@@ -2756,7 +2754,7 @@
         <v>49</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13">
         <f t="shared" si="10"/>
@@ -3404,11 +3402,6 @@
       </c>
       <c r="I22" s="7" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3521,7 +3514,7 @@
         <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -3618,7 +3611,7 @@
         <v>174</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F2" t="s">
         <v>178</v>
@@ -3701,13 +3694,13 @@
         <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,7 +3719,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -3740,7 +3733,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3784,7 +3777,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -3801,7 +3794,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
         <v>184</v>

</xml_diff>